<commit_message>
updated test-plan and bug-list
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -49,7 +49,21 @@
     <t>Peter</t>
   </si>
   <si>
-    <t>After pressing the spacebar once, holding it down while moving the character left or right disables the main character's animation temporarily.</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">After pressing the spacebar once, holding it down while moving the character left or right disables the main character's animation temporarily. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>[FIXED]</t>
+    </r>
   </si>
   <si>
     <t>The character's walking animation should always be visible, regardless of whether the spacebar is being held down.</t>
@@ -156,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -180,6 +194,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,11 +462,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="33.0" customHeight="1">
-      <c r="B4" s="7" t="s">
+    <row r="4" ht="39.0" customHeight="1">
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="7" t="s">

</xml_diff>